<commit_message>
Added support for a ControlStrategy for Producers
</commit_message>
<xml_diff>
--- a/data/infrastructure_4.xlsx
+++ b/data/infrastructure_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthijssenef\PycharmProjects\excel-2-esdl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448F36A3-D35D-48CF-AB8E-ADDB7F4A2DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662B6F91-CEDE-4C50-922B-0F77AEDAAA48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="4515" windowWidth="43530" windowHeight="14265" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="2400" windowWidth="24150" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
   <si>
     <t>ID</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t>MC_Profile_ID</t>
+  </si>
+  <si>
+    <t>CS_Curt_MaxPower</t>
   </si>
 </sst>
 </file>
@@ -707,7 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFEC4E92-53F5-402E-96D4-F7619F5A0534}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -909,11 +912,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -929,9 +930,11 @@
     <col min="17" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -993,13 +996,19 @@
         <v>106</v>
       </c>
       <c r="U1" t="s">
+        <v>112</v>
+      </c>
+      <c r="V1" t="s">
+        <v>118</v>
+      </c>
+      <c r="W1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1040,7 +1049,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1133,9 +1142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E59E50-3AA1-4991-AB07-24A7E9585BA0}">
   <dimension ref="A1:Y3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Implement behaviour specification for Conversion assets, add extra InPort/OutPort for Conversion assets
</commit_message>
<xml_diff>
--- a/data/infrastructure_4.xlsx
+++ b/data/infrastructure_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthijssenef\PycharmProjects\excel-2-esdl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662B6F91-CEDE-4C50-922B-0F77AEDAAA48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895102B2-8C36-46A2-9B84-B2FBAC6CE5F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="2400" windowWidth="24150" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-4050" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="132">
   <si>
     <t>ID</t>
   </si>
@@ -390,16 +390,61 @@
   </si>
   <si>
     <t>CS_Curt_MaxPower</t>
+  </si>
+  <si>
+    <t>Behaviour</t>
+  </si>
+  <si>
+    <t>InputOutputRelation</t>
+  </si>
+  <si>
+    <t>IOR_Port1</t>
+  </si>
+  <si>
+    <t>IOR_Port2</t>
+  </si>
+  <si>
+    <t>IOR_Port3</t>
+  </si>
+  <si>
+    <t>IOR_Port4</t>
+  </si>
+  <si>
+    <t>IOR_Port5</t>
+  </si>
+  <si>
+    <t>IOR_MainPort_ID</t>
+  </si>
+  <si>
+    <t>IOR_Port1_Ratio</t>
+  </si>
+  <si>
+    <t>IOR_Port2_Ratio</t>
+  </si>
+  <si>
+    <t>IOR_Port3_Ratio</t>
+  </si>
+  <si>
+    <t>IOR_Port4_Ratio</t>
+  </si>
+  <si>
+    <t>IOR_Port5_Ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1140,7 +1185,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E59E50-3AA1-4991-AB07-24A7E9585BA0}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1161,9 +1206,11 @@
     <col min="21" max="21" width="16" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1239,8 +1286,44 @@
       <c r="Y1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -1295,8 +1378,20 @@
       <c r="Y2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -1347,6 +1442,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>